<commit_message>
Changed 2d calculations to 3d
</commit_message>
<xml_diff>
--- a/Documents/TestPlan.xlsx
+++ b/Documents/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horse\source\repos\LocationTriggering\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F499F7-F39E-4729-AC8D-12D88C924820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96089536-6885-45CB-8480-53D1C64B6DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -613,6 +613,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -622,26 +640,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -651,9 +654,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -941,7 +941,7 @@
   <dimension ref="A4:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:K7"/>
+      <selection activeCell="C14" sqref="C14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,22 +966,22 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="3" t="s">
         <v>51</v>
       </c>
@@ -990,24 +990,24 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="29" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="G7" s="29" t="s">
+      <c r="E7" s="27"/>
+      <c r="G7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="29" t="s">
+      <c r="H7" s="35"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="31"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -1034,10 +1034,10 @@
       <c r="I8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="33"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -1065,8 +1065,8 @@
       <c r="I9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="33"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
@@ -1094,10 +1094,10 @@
       <c r="I10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="33"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
@@ -1125,10 +1125,10 @@
       <c r="I11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="35" t="s">
+      <c r="J11" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="33"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -1156,8 +1156,8 @@
       <c r="I12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="35"/>
-      <c r="K12" s="33"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="29"/>
     </row>
     <row r="13" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
@@ -1185,8 +1185,8 @@
       <c r="I13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="33"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
@@ -1214,8 +1214,8 @@
       <c r="I14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
@@ -1243,12 +1243,17 @@
       <c r="I15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
     </row>
     <row r="16" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J15:K15"/>
@@ -1258,11 +1263,6 @@
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1274,7 +1274,7 @@
   <dimension ref="A4:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C12" sqref="C12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,22 +1298,22 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="15" t="s">
         <v>2</v>
       </c>
@@ -1322,24 +1322,24 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="29" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="G7" s="39" t="s">
+      <c r="E7" s="27"/>
+      <c r="G7" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39" t="s">
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="39"/>
+      <c r="K7" s="36"/>
     </row>
     <row r="8" spans="1:11" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
@@ -1366,10 +1366,10 @@
       <c r="I8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="J8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="37"/>
+      <c r="K8" s="38"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
@@ -1393,8 +1393,8 @@
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="16"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="37"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
@@ -1418,8 +1418,8 @@
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="16"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="37"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="11" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
@@ -1443,8 +1443,8 @@
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="37"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="38"/>
     </row>
     <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
@@ -1468,23 +1468,23 @@
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="16"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="37"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1496,7 +1496,7 @@
   <dimension ref="A4:K18"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:G17"/>
+      <selection activeCell="C11" sqref="C11:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,22 +1520,22 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1544,24 +1544,24 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="29" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="G7" s="39" t="s">
+      <c r="E7" s="27"/>
+      <c r="G7" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39" t="s">
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="39"/>
+      <c r="K7" s="36"/>
     </row>
     <row r="8" spans="1:11" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -1588,10 +1588,10 @@
       <c r="I8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="36" t="s">
+      <c r="J8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="37"/>
+      <c r="K8" s="38"/>
     </row>
     <row r="9" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -1615,8 +1615,8 @@
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="37"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
@@ -1640,8 +1640,8 @@
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="37"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="11" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
@@ -1665,8 +1665,8 @@
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="37"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="38"/>
     </row>
     <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -1690,8 +1690,8 @@
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="37"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
@@ -1715,8 +1715,8 @@
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="37"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="38"/>
     </row>
     <row r="14" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
@@ -1740,8 +1740,8 @@
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="37"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="38"/>
     </row>
     <row r="15" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
@@ -1765,8 +1765,8 @@
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="37"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
@@ -1790,7 +1790,7 @@
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="32"/>
+      <c r="J16" s="28"/>
       <c r="K16" s="40"/>
     </row>
     <row r="17" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1815,16 +1815,509 @@
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="32"/>
+      <c r="J17" s="28"/>
       <c r="K17" s="40"/>
     </row>
     <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07DFB7-1DE4-48D7-9A1C-68A3201B0612}">
+  <dimension ref="A4:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="G7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="36"/>
+    </row>
+    <row r="8" spans="1:11" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="38"/>
+    </row>
+    <row r="9" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="38"/>
+    </row>
+    <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G7:I7"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80A2EA8-97F7-4E6B-80A8-82F23FE2CBCE}">
+  <dimension ref="A4:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="G7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="36"/>
+    </row>
+    <row r="8" spans="1:11" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="38"/>
+    </row>
+    <row r="9" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="38"/>
+    </row>
+    <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="9">
+        <v>44102</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="J10:K10"/>
@@ -1841,497 +2334,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07DFB7-1DE4-48D7-9A1C-68A3201B0612}">
-  <dimension ref="A4:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="G7" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="39"/>
-    </row>
-    <row r="8" spans="1:11" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="37"/>
-    </row>
-    <row r="9" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="37"/>
-    </row>
-    <row r="10" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="37"/>
-    </row>
-    <row r="11" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="37"/>
-    </row>
-    <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="37"/>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-  </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80A2EA8-97F7-4E6B-80A8-82F23FE2CBCE}">
-  <dimension ref="A4:K15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="G7" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="39"/>
-    </row>
-    <row r="8" spans="1:11" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="37"/>
-    </row>
-    <row r="9" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="37"/>
-    </row>
-    <row r="10" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="37"/>
-    </row>
-    <row r="11" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="37"/>
-    </row>
-    <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="37"/>
-    </row>
-    <row r="13" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="37"/>
-    </row>
-    <row r="14" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="9">
-        <v>44102</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="37"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>